<commit_message>
Final updates for project 04
</commit_message>
<xml_diff>
--- a/Team_Bruno_Christian_Daniel_Jack_Report.xlsx
+++ b/Team_Bruno_Christian_Daniel_Jack_Report.xlsx
@@ -19,14 +19,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="276">
+  <si>
+    <t>Initials</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>GitHub Username</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>dbarry@stevens.edu</t>
+  </si>
+  <si>
+    <t>DanJBarry</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Chaneski</t>
+  </si>
+  <si>
+    <t>cchanesk@stevens.edu</t>
+  </si>
+  <si>
+    <t>XiliferVinine</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Engel</t>
+  </si>
+  <si>
+    <t>jengel@stevens.edu</t>
+  </si>
+  <si>
+    <t>engeljb10</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Salgado</t>
+  </si>
+  <si>
+    <t>bsalgado@stevens.edu</t>
+  </si>
   <si>
     <t>Sprint</t>
   </si>
   <si>
+    <t>bsalgado98</t>
+  </si>
+  <si>
     <t>Story ID</t>
   </si>
   <si>
+    <t>GitHub Repository:</t>
+  </si>
+  <si>
     <t>Story Name</t>
   </si>
   <si>
@@ -36,123 +114,45 @@
     <t>Status</t>
   </si>
   <si>
+    <t>https://github.com/bsalgado98/SSW555-GEDCOM.git</t>
+  </si>
+  <si>
     <t>US01</t>
   </si>
   <si>
-    <t>Initials</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>GitHub Username</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
     <t>Dates before current date</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
-    <t>Barry</t>
-  </si>
-  <si>
-    <t>dbarry@stevens.edu</t>
-  </si>
-  <si>
-    <t>DanJBarry</t>
-  </si>
-  <si>
     <t>US02</t>
   </si>
   <si>
-    <t>Christian</t>
-  </si>
-  <si>
     <t>Birth before marriage</t>
   </si>
   <si>
-    <t>Chaneski</t>
-  </si>
-  <si>
-    <t>BS</t>
-  </si>
-  <si>
-    <t>cchanesk@stevens.edu</t>
-  </si>
-  <si>
-    <t>XiliferVinine</t>
-  </si>
-  <si>
     <t>US03</t>
   </si>
   <si>
-    <t>JE</t>
-  </si>
-  <si>
     <t>Birth before death</t>
   </si>
   <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Engel</t>
-  </si>
-  <si>
-    <t>jengel@stevens.edu</t>
-  </si>
-  <si>
-    <t>engeljb10</t>
-  </si>
-  <si>
     <t>US04</t>
   </si>
   <si>
     <t>Marriage before divorce</t>
   </si>
   <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Salgado</t>
-  </si>
-  <si>
-    <t>bsalgado@stevens.edu</t>
-  </si>
-  <si>
     <t>US05</t>
   </si>
   <si>
-    <t>bsalgado98</t>
-  </si>
-  <si>
     <t>Marriage before death</t>
   </si>
   <si>
-    <t>GitHub Repository:</t>
-  </si>
-  <si>
     <t>US06</t>
   </si>
   <si>
-    <t>https://github.com/bsalgado98/SSW555-GEDCOM.git</t>
-  </si>
-  <si>
     <t>Divorce before death</t>
   </si>
   <si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>Split NAME string for each individual to get last name</t>
+  </si>
+  <si>
+    <t>T16.03</t>
   </si>
   <si>
     <t>Check if all strings are equal</t>
@@ -1016,11 +1019,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1350533791"/>
-        <c:axId val="754164056"/>
+        <c:axId val="109704150"/>
+        <c:axId val="722492605"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1350533791"/>
+        <c:axId val="109704150"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,10 +1038,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="754164056"/>
+        <c:crossAx val="722492605"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="754164056"/>
+        <c:axId val="722492605"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1072,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350533791"/>
+        <c:crossAx val="109704150"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1125,11 +1128,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="451601048"/>
-        <c:axId val="902931677"/>
+        <c:axId val="572846321"/>
+        <c:axId val="901790620"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451601048"/>
+        <c:axId val="572846321"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,10 +1147,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="902931677"/>
+        <c:crossAx val="901790620"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="902931677"/>
+        <c:axId val="901790620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1181,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451601048"/>
+        <c:crossAx val="572846321"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1849,19 +1852,19 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1888,80 +1891,80 @@
     <row r="2" ht="12.75" customHeight="1"/>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1"/>
     <row r="9" ht="12.75" customHeight="1">
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1"/>
@@ -2986,19 +2989,19 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -3027,16 +3030,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -3044,16 +3047,16 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
@@ -3061,16 +3064,16 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
@@ -3078,16 +3081,16 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
@@ -3095,16 +3098,16 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3112,16 +3115,16 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -3135,10 +3138,10 @@
         <v>46</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
@@ -3152,7 +3155,7 @@
         <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>49</v>
@@ -3169,7 +3172,7 @@
         <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>49</v>
@@ -3186,7 +3189,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>49</v>
@@ -3203,10 +3206,10 @@
         <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
@@ -3220,7 +3223,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>49</v>
@@ -3237,7 +3240,7 @@
         <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>49</v>
@@ -3254,7 +3257,7 @@
         <v>61</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>49</v>
@@ -3271,7 +3274,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>49</v>
@@ -3288,7 +3291,7 @@
         <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>49</v>
@@ -4489,7 +4492,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>166</v>
@@ -12707,16 +12710,16 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>102</v>
@@ -12736,16 +12739,16 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2">
         <v>10.0</v>
@@ -12775,7 +12778,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I4" s="10"/>
     </row>
@@ -12787,7 +12790,7 @@
         <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I5" s="10"/>
     </row>
@@ -12799,7 +12802,7 @@
         <v>113</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I6" s="10"/>
     </row>
@@ -12809,16 +12812,16 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2">
         <v>10.0</v>
@@ -12848,7 +12851,7 @@
         <v>115</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I10" s="10"/>
     </row>
@@ -12860,7 +12863,7 @@
         <v>117</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I11" s="10"/>
     </row>
@@ -12872,7 +12875,7 @@
         <v>119</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I12" s="10"/>
     </row>
@@ -12882,16 +12885,16 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2">
         <v>10.0</v>
@@ -12921,7 +12924,7 @@
         <v>115</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I16" s="10"/>
     </row>
@@ -12933,7 +12936,7 @@
         <v>122</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I17" s="10"/>
     </row>
@@ -12945,7 +12948,7 @@
         <v>124</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I18" s="10"/>
     </row>
@@ -12955,16 +12958,16 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E20" s="2">
         <v>10.0</v>
@@ -12993,7 +12996,7 @@
         <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I22" s="10"/>
     </row>
@@ -13005,7 +13008,7 @@
         <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I23" s="10"/>
     </row>
@@ -13017,7 +13020,7 @@
         <v>130</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I24" s="10"/>
     </row>
@@ -13026,16 +13029,16 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E26" s="2">
         <v>10.0</v>
@@ -13064,7 +13067,7 @@
         <v>126</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I28" s="10"/>
     </row>
@@ -13076,7 +13079,7 @@
         <v>122</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I29" s="10"/>
     </row>
@@ -13088,7 +13091,7 @@
         <v>134</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I30" s="10"/>
     </row>
@@ -13097,16 +13100,16 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E32" s="2">
         <v>22.0</v>
@@ -13135,7 +13138,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I34" s="10"/>
     </row>
@@ -13147,7 +13150,7 @@
         <v>122</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I35" s="10"/>
     </row>
@@ -13159,7 +13162,7 @@
         <v>138</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I36" s="10"/>
     </row>
@@ -13174,10 +13177,10 @@
         <v>46</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E38" s="2">
         <v>10.0</v>
@@ -13206,7 +13209,7 @@
         <v>140</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I40" s="10"/>
     </row>
@@ -13218,7 +13221,7 @@
         <v>142</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I41" s="10"/>
     </row>
@@ -13230,7 +13233,7 @@
         <v>144</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I42" s="10"/>
     </row>
@@ -13242,7 +13245,7 @@
         <v>146</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I43" s="10"/>
     </row>
@@ -13257,10 +13260,10 @@
         <v>55</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E45" s="2">
         <v>20.0</v>
@@ -13289,7 +13292,7 @@
         <v>126</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I47" s="10"/>
     </row>
@@ -13301,7 +13304,7 @@
         <v>149</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I48" s="10"/>
     </row>
@@ -13313,7 +13316,7 @@
         <v>151</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="I49" s="10"/>
     </row>
@@ -17197,16 +17200,16 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>102</v>
@@ -17232,7 +17235,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>49</v>
@@ -17282,7 +17285,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>49</v>
@@ -17332,7 +17335,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>49</v>
@@ -17375,7 +17378,7 @@
         <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>49</v>
@@ -17418,7 +17421,7 @@
         <v>196</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>49</v>
@@ -17468,7 +17471,7 @@
         <v>203</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>49</v>
@@ -17518,7 +17521,7 @@
         <v>63</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>49</v>
@@ -17560,7 +17563,7 @@
         <v>65</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>49</v>
@@ -17592,8 +17595,11 @@
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
+      <c r="A45" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="B45" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
@@ -18598,16 +18604,16 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>102</v>
@@ -19647,16 +19653,16 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>102</v>
@@ -20699,13 +20705,13 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -20733,68 +20739,68 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -20805,7 +20811,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
@@ -20816,7 +20822,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
@@ -20827,7 +20833,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
@@ -20838,7 +20844,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
@@ -20849,7 +20855,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
@@ -20860,7 +20866,7 @@
         <v>57</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
@@ -20871,7 +20877,7 @@
         <v>59</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
@@ -20882,7 +20888,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
@@ -20893,7 +20899,7 @@
         <v>63</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
@@ -20904,7 +20910,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
@@ -20915,7 +20921,7 @@
         <v>67</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
@@ -20926,7 +20932,7 @@
         <v>69</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
@@ -20937,7 +20943,7 @@
         <v>71</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
@@ -20948,7 +20954,7 @@
         <v>73</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
@@ -20959,7 +20965,7 @@
         <v>75</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
@@ -20970,7 +20976,7 @@
         <v>77</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
@@ -20981,7 +20987,7 @@
         <v>79</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
@@ -20992,7 +20998,7 @@
         <v>81</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
@@ -21003,7 +21009,7 @@
         <v>83</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
@@ -21014,7 +21020,7 @@
         <v>85</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
@@ -21025,7 +21031,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
@@ -21036,7 +21042,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
@@ -21047,7 +21053,7 @@
         <v>91</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -21058,7 +21064,7 @@
         <v>93</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
@@ -21069,95 +21075,95 @@
         <v>95</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B34" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B35" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B36" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B37" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
@@ -21168,7 +21174,7 @@
         <v>97</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
@@ -21179,7 +21185,7 @@
         <v>99</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
@@ -21190,7 +21196,7 @@
         <v>101</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">

</xml_diff>